<commit_message>
updated shot distance data
</commit_message>
<xml_diff>
--- a/nba_scoring/shot_distance.xlsx
+++ b/nba_scoring/shot_distance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielmelmed/git_repos/charts_gratia_chartis/nba_scoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56CE9565-0F65-3D4E-9F04-5650D3640720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE71A754-36BB-9A45-B026-3F6EDF77DB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{2E417CE6-143A-E341-B1E9-4860D2389AEA}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,10 +493,10 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="D2" s="3">
-        <v>0.20699999999999999</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="E2" s="3">
-        <v>9.4E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="F2" s="3">
         <v>5.0999999999999997E-2</v>

</xml_diff>